<commit_message>
Updated Readme file and other fixes
</commit_message>
<xml_diff>
--- a/RhineSignupBDD/src/test/resources/Excel/testdata.xlsx
+++ b/RhineSignupBDD/src/test/resources/Excel/testdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajayb\Eclipse-Project\RhineSignupBDD\src\test\resources\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajayb\RhineAutomationProject\RhineSignupBDD\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C575A730-5B03-467C-8488-04CA9C9DA692}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{507319EB-51EA-4F6D-BAD2-690B1B2CC333}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{67C2AAF6-E234-4376-88A9-4BD48F593E90}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{67C2AAF6-E234-4376-88A9-4BD48F593E90}"/>
   </bookViews>
   <sheets>
     <sheet name="SignUpSteps" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>postcode</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>url</t>
+  </si>
+  <si>
+    <t>ramanarora@abc.com.au</t>
   </si>
 </sst>
 </file>
@@ -506,11 +509,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC45BA88-6DDA-44FD-A4A9-E8C0EFB2B3A2}">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="11" max="11" width="9.76171875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.29296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.17578125" customWidth="1"/>
     <col min="16" max="16" width="16.3515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="22.29296875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="21.87890625" bestFit="1" customWidth="1"/>
@@ -624,6 +631,9 @@
       <c r="M2" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="N2" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="O2" t="s">
         <v>29</v>
       </c>
@@ -651,6 +661,7 @@
     <hyperlink ref="M2" r:id="rId1" xr:uid="{48D6030D-281B-43DA-B497-8FEF9F4427C5}"/>
     <hyperlink ref="U2" r:id="rId2" xr:uid="{5140B2C9-8E40-47D2-A760-51B33A9AFE75}"/>
     <hyperlink ref="A2" r:id="rId3" xr:uid="{33618F51-B3F4-4570-A7E1-0D96EE9E201B}"/>
+    <hyperlink ref="N2" r:id="rId4" xr:uid="{3C318894-EF32-46F5-B277-5F7ECD64D35F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>